<commit_message>
Updated members and addresses 2021
</commit_message>
<xml_diff>
--- a/data/lab_members_addresses.xlsx
+++ b/data/lab_members_addresses.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ido Bar\Documents\Github\lab_members\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau.sharepoint.com/sites/SustainableFoodProductionGroup/Shared Documents/General/lab_members/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87D8CB8-1F75-4A69-9DF7-E9E2E6BC9830}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{E87D8CB8-1F75-4A69-9DF7-E9E2E6BC9830}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC6A37DF-E843-4528-99BB-048410A6EDC6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9255" xr2:uid="{0406F0C8-C7E6-457B-BAD9-300B5038A677}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0406F0C8-C7E6-457B-BAD9-300B5038A677}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2021" sheetId="1" r:id="rId1"/>
+    <sheet name="2018" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +24,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -41,6 +46,9 @@
     <t>Ido Bar</t>
   </si>
   <si>
+    <t>Givat Ada, Israel</t>
+  </si>
+  <si>
     <t>Kazbek Dyussembayev</t>
   </si>
   <si>
@@ -50,12 +58,18 @@
     <t>Andres Godwin Sajise</t>
   </si>
   <si>
+    <t>UPLB Laguna, Philippines</t>
+  </si>
+  <si>
     <t>Marzia Bilkiss</t>
   </si>
   <si>
     <t>Tangail, Bangladesh</t>
   </si>
   <si>
+    <t>Sam (Prabhakaran) Thanjavur Sambasivam</t>
+  </si>
+  <si>
     <t>Chennai, Tamilnadu, India</t>
   </si>
   <si>
@@ -89,19 +103,28 @@
     <t>Hartley Wintney, Hampshire, UK</t>
   </si>
   <si>
-    <t>UPLB Laguna, Philippines</t>
-  </si>
-  <si>
     <t>Shane (Zi Wei) Zhou</t>
   </si>
   <si>
-    <t>Sam (Prabhakaran) Thanjavur Sambasivam</t>
-  </si>
-  <si>
     <t>Nantong, Jiangsu, China</t>
   </si>
   <si>
-    <t>Givat Ada, Israel</t>
+    <t>Rachel Diva Soh</t>
+  </si>
+  <si>
+    <t>Jakarta, Indonesia</t>
+  </si>
+  <si>
+    <t>Melody Christie</t>
+  </si>
+  <si>
+    <t>Alberton, Canada</t>
+  </si>
+  <si>
+    <t>Jeremy Brownlie</t>
+  </si>
+  <si>
+    <t>Canberra, Australia</t>
   </si>
 </sst>
 </file>
@@ -157,11 +180,22 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ECEF8CCD-7D66-412B-82A5-6A174A374E72}" name="Table1" displayName="Table1" ref="A1:B12" totalsRowShown="0">
-  <autoFilter ref="A1:B12" xr:uid="{61704248-9450-4A3F-A22E-D43AC41A2786}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ECEF8CCD-7D66-412B-82A5-6A174A374E72}" name="Table1" displayName="Table1" ref="A1:B10" totalsRowShown="0">
+  <autoFilter ref="A1:B10" xr:uid="{61704248-9450-4A3F-A22E-D43AC41A2786}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1B25737D-01FD-4913-B71A-8582AA1E0E9E}" name="Name"/>
     <tableColumn id="2" xr3:uid="{D653BEAC-5602-4A54-88E4-28E70751F17B}" name="Address"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C1E1DBCB-B323-4BD0-9BA3-9BE1465BD868}" name="Table13" displayName="Table13" ref="A1:B15" totalsRowShown="0">
+  <autoFilter ref="A1:B15" xr:uid="{61704248-9450-4A3F-A22E-D43AC41A2786}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{A64DC093-3776-4B4B-B8DD-B9A609ADA46D}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{7DD9AFF2-F8D0-41CA-BACF-3E3E91F1ACF4}" name="Address"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -464,19 +498,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FFB128-7185-45DB-9774-8BE493C2C42E}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -484,92 +518,76 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -578,4 +596,449 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DB2185-0E3C-4BE5-BD3F-1BFF659687AF}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010042F0EEFC51374E449569A1D7EE9E03E1" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f6fe47d03a198c1fbfb51d8f6832cd45">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b6e6b88c-8d12-40de-97ca-53d6a0947b55" xmlns:ns3="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3205387083a8711250c9ab547032f400" ns2:_="" ns3:_="">
+    <xsd:import namespace="b6e6b88c-8d12-40de-97ca-53d6a0947b55"/>
+    <xsd:import namespace="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b6e6b88c-8d12-40de-97ca-53d6a0947b55" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="10" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="14" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255">
+      <UserInfo>
+        <DisplayName>Marzia Bilkiss</DisplayName>
+        <AccountId>14</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ZiWei Zhou</DisplayName>
+        <AccountId>20</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Chat Kanchana-Udomkan</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Gurpreet Khalsa</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeremy Brownlie</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Melody Christie</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Prabhakaran Thanjavur Sambasivam</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Rebecca Ford</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>matin ghaheri</DisplayName>
+        <AccountId>27</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60A4FA7D-2332-467E-A61F-E24FCB3AB047}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b6e6b88c-8d12-40de-97ca-53d6a0947b55"/>
+    <ds:schemaRef ds:uri="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC31AB97-46D5-4FEB-9391-03C657BC4DCE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27287F92-5990-45D2-9430-8EC47D151C4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Parse countries and country codes from original address
</commit_message>
<xml_diff>
--- a/data/lab_members_addresses.xlsx
+++ b/data/lab_members_addresses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau.sharepoint.com/sites/SustainableFoodProductionGroup/Shared Documents/General/lab_members/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{E87D8CB8-1F75-4A69-9DF7-E9E2E6BC9830}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC6A37DF-E843-4528-99BB-048410A6EDC6}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{E87D8CB8-1F75-4A69-9DF7-E9E2E6BC9830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B05195AF-9F01-4494-9A41-FB20B87D8616}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0406F0C8-C7E6-457B-BAD9-300B5038A677}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{0406F0C8-C7E6-457B-BAD9-300B5038A677}"/>
   </bookViews>
   <sheets>
     <sheet name="2021" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -49,6 +49,57 @@
     <t>Givat Ada, Israel</t>
   </si>
   <si>
+    <t>Sam (Prabhakaran) Thanjavur Sambasivam</t>
+  </si>
+  <si>
+    <t>Chennai, Tamilnadu, India</t>
+  </si>
+  <si>
+    <t>Chat Kanchana-Udomkan</t>
+  </si>
+  <si>
+    <t>Kanchanaburi, Thailand</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Nathan, QLD, Australia</t>
+  </si>
+  <si>
+    <t>Rebecca Ford</t>
+  </si>
+  <si>
+    <t>Hartley Wintney, Hampshire, UK</t>
+  </si>
+  <si>
+    <t>Shane (Zi Wei) Zhou</t>
+  </si>
+  <si>
+    <t>Nantong, Jiangsu, China</t>
+  </si>
+  <si>
+    <t>Rachel Diva Soh</t>
+  </si>
+  <si>
+    <t>Jakarta, Indonesia</t>
+  </si>
+  <si>
+    <t>Melody Christie</t>
+  </si>
+  <si>
+    <t>Alberton, Canada</t>
+  </si>
+  <si>
+    <t>Jeremy Brownlie</t>
+  </si>
+  <si>
+    <t>Canberra, Australia</t>
+  </si>
+  <si>
+    <t>Gurpreet Singh Khalsa</t>
+  </si>
+  <si>
     <t>Kazbek Dyussembayev</t>
   </si>
   <si>
@@ -67,18 +118,6 @@
     <t>Tangail, Bangladesh</t>
   </si>
   <si>
-    <t>Sam (Prabhakaran) Thanjavur Sambasivam</t>
-  </si>
-  <si>
-    <t>Chennai, Tamilnadu, India</t>
-  </si>
-  <si>
-    <t>Chat Kanchana-Udomkan</t>
-  </si>
-  <si>
-    <t>Kanchanaburi, Thailand</t>
-  </si>
-  <si>
     <t>Usana Nantawan</t>
   </si>
   <si>
@@ -91,40 +130,7 @@
     <t>Tehran, Iran</t>
   </si>
   <si>
-    <t>Lab</t>
-  </si>
-  <si>
-    <t>Nathan, QLD, Australia</t>
-  </si>
-  <si>
-    <t>Rebecca Ford</t>
-  </si>
-  <si>
-    <t>Hartley Wintney, Hampshire, UK</t>
-  </si>
-  <si>
-    <t>Shane (Zi Wei) Zhou</t>
-  </si>
-  <si>
-    <t>Nantong, Jiangsu, China</t>
-  </si>
-  <si>
-    <t>Rachel Diva Soh</t>
-  </si>
-  <si>
-    <t>Jakarta, Indonesia</t>
-  </si>
-  <si>
-    <t>Melody Christie</t>
-  </si>
-  <si>
-    <t>Alberton, Canada</t>
-  </si>
-  <si>
-    <t>Jeremy Brownlie</t>
-  </si>
-  <si>
-    <t>Canberra, Australia</t>
+    <t>Jammu, India</t>
   </si>
 </sst>
 </file>
@@ -180,8 +186,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ECEF8CCD-7D66-412B-82A5-6A174A374E72}" name="Table1" displayName="Table1" ref="A1:B10" totalsRowShown="0">
-  <autoFilter ref="A1:B10" xr:uid="{61704248-9450-4A3F-A22E-D43AC41A2786}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ECEF8CCD-7D66-412B-82A5-6A174A374E72}" name="Table1" displayName="Table1" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11" xr:uid="{61704248-9450-4A3F-A22E-D43AC41A2786}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{1B25737D-01FD-4913-B71A-8582AA1E0E9E}" name="Name"/>
     <tableColumn id="2" xr3:uid="{D653BEAC-5602-4A54-88E4-28E70751F17B}" name="Address"/>
@@ -498,19 +504,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FFB128-7185-45DB-9774-8BE493C2C42E}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -518,7 +524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -526,68 +532,76 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
+      <c r="B11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -606,13 +620,13 @@
       <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -620,7 +634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -628,108 +642,108 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -741,6 +755,74 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255">
+      <UserInfo>
+        <DisplayName>Marzia Bilkiss</DisplayName>
+        <AccountId>14</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>ZiWei Zhou</DisplayName>
+        <AccountId>20</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Chat Kanchana-Udomkan</DisplayName>
+        <AccountId>12</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Gurpreet Khalsa</DisplayName>
+        <AccountId>28</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Jeremy Brownlie</DisplayName>
+        <AccountId>19</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Melody Christie</DisplayName>
+        <AccountId>21</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Prabhakaran Thanjavur Sambasivam</DisplayName>
+        <AccountId>15</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Rebecca Ford</DisplayName>
+        <AccountId>7</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>matin ghaheri</DisplayName>
+        <AccountId>27</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ido Bar</DisplayName>
+        <AccountId>13</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010042F0EEFC51374E449569A1D7EE9E03E1" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f6fe47d03a198c1fbfb51d8f6832cd45">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b6e6b88c-8d12-40de-97ca-53d6a0947b55" xmlns:ns3="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3205387083a8711250c9ab547032f400" ns2:_="" ns3:_="">
     <xsd:import namespace="b6e6b88c-8d12-40de-97ca-53d6a0947b55"/>
@@ -943,70 +1025,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255">
-      <UserInfo>
-        <DisplayName>Marzia Bilkiss</DisplayName>
-        <AccountId>14</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>ZiWei Zhou</DisplayName>
-        <AccountId>20</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Chat Kanchana-Udomkan</DisplayName>
-        <AccountId>12</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Gurpreet Khalsa</DisplayName>
-        <AccountId>28</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Jeremy Brownlie</DisplayName>
-        <AccountId>19</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Melody Christie</DisplayName>
-        <AccountId>21</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Prabhakaran Thanjavur Sambasivam</DisplayName>
-        <AccountId>15</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Rebecca Ford</DisplayName>
-        <AccountId>7</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>matin ghaheri</DisplayName>
-        <AccountId>27</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC31AB97-46D5-4FEB-9391-03C657BC4DCE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27287F92-5990-45D2-9430-8EC47D151C4F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60A4FA7D-2332-467E-A61F-E24FCB3AB047}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1023,22 +1060,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC31AB97-46D5-4FEB-9391-03C657BC4DCE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27287F92-5990-45D2-9430-8EC47D151C4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated new students details
</commit_message>
<xml_diff>
--- a/data/lab_members_addresses.xlsx
+++ b/data/lab_members_addresses.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25415"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau.sharepoint.com/sites/SustainableFoodProductionGroup/Shared Documents/General/lab_members/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{E87D8CB8-1F75-4A69-9DF7-E9E2E6BC9830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B05195AF-9F01-4494-9A41-FB20B87D8616}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{E87D8CB8-1F75-4A69-9DF7-E9E2E6BC9830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66A8CDFA-5F55-4748-A1B0-BEBA142B4376}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{0406F0C8-C7E6-457B-BAD9-300B5038A677}"/>
+    <workbookView xWindow="8460" yWindow="900" windowWidth="17610" windowHeight="14220" xr2:uid="{0406F0C8-C7E6-457B-BAD9-300B5038A677}"/>
   </bookViews>
   <sheets>
-    <sheet name="2021" sheetId="1" r:id="rId1"/>
-    <sheet name="2018" sheetId="2" r:id="rId2"/>
+    <sheet name="2022" sheetId="3" r:id="rId1"/>
+    <sheet name="2021" sheetId="1" r:id="rId2"/>
+    <sheet name="2018" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -28,14 +29,33 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={C0F18B8E-F82B-4641-8E03-2514981C1209}</author>
+  </authors>
+  <commentList>
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{C0F18B8E-F82B-4641-8E03-2514981C1209}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Fawad Ali</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -88,18 +108,66 @@
     <t>Melody Christie</t>
   </si>
   <si>
+    <t>Prince Edward Island, Canada</t>
+  </si>
+  <si>
+    <t>Jeremy Brownlie</t>
+  </si>
+  <si>
+    <t>Canberra, Australia</t>
+  </si>
+  <si>
+    <t>Gurpreet Singh Khalsa</t>
+  </si>
+  <si>
+    <t>Jammu, India</t>
+  </si>
+  <si>
+    <t>Matin Ghaheri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isfahan, Iran </t>
+  </si>
+  <si>
+    <t>Henrietta Soi</t>
+  </si>
+  <si>
+    <t>Nairobi, Kenya</t>
+  </si>
+  <si>
+    <t>Fawad Ali</t>
+  </si>
+  <si>
+    <t>Faisalabad-Punjab Pakistan</t>
+  </si>
+  <si>
+    <t>Moutoshi Chakraborty</t>
+  </si>
+  <si>
+    <t>Naogaon, Bangladesh</t>
+  </si>
+  <si>
+    <t>Hayley Wilson</t>
+  </si>
+  <si>
+    <t>Melbourne and Tamworth, Australia</t>
+  </si>
+  <si>
+    <t>Joshua Lomax</t>
+  </si>
+  <si>
+    <t>Cairns, Autralia</t>
+  </si>
+  <si>
+    <t>Mahmuda Binte Monsur</t>
+  </si>
+  <si>
+    <t>Tangail, Dhaka, Bangladesh</t>
+  </si>
+  <si>
     <t>Alberton, Canada</t>
   </si>
   <si>
-    <t>Jeremy Brownlie</t>
-  </si>
-  <si>
-    <t>Canberra, Australia</t>
-  </si>
-  <si>
-    <t>Gurpreet Singh Khalsa</t>
-  </si>
-  <si>
     <t>Kazbek Dyussembayev</t>
   </si>
   <si>
@@ -128,16 +196,13 @@
   </si>
   <si>
     <t>Tehran, Iran</t>
-  </si>
-  <si>
-    <t>Jammu, India</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,7 +250,24 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Fawad Ali" id="{481E44AB-5366-DD46-8FD7-F0A6B87DC6FA}" userId="S::fawad.ali@griffith.edu.au::934a7e08-d53e-445b-adea-23820242cb95" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{3319C2E2-5B2F-4DA2-9240-9F6F956D2D44}" name="Table14" displayName="Table14" ref="A1:B16" totalsRowShown="0">
+  <autoFilter ref="A1:B16" xr:uid="{61704248-9450-4A3F-A22E-D43AC41A2786}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{12EA01B7-5FD4-495C-84C4-8CB128CEA401}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{CC8A1CF0-7BD9-46F4-86F0-DBF1C7CD034C}" name="Address"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ECEF8CCD-7D66-412B-82A5-6A174A374E72}" name="Table1" displayName="Table1" ref="A1:B11" totalsRowShown="0">
   <autoFilter ref="A1:B11" xr:uid="{61704248-9450-4A3F-A22E-D43AC41A2786}"/>
   <tableColumns count="2">
@@ -196,7 +278,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C1E1DBCB-B323-4BD0-9BA3-9BE1465BD868}" name="Table13" displayName="Table13" ref="A1:B15" totalsRowShown="0">
   <autoFilter ref="A1:B15" xr:uid="{61704248-9450-4A3F-A22E-D43AC41A2786}"/>
   <tableColumns count="2">
@@ -502,21 +584,196 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A14" dT="2022-06-23T06:28:46.62" personId="{481E44AB-5366-DD46-8FD7-F0A6B87DC6FA}" id="{C0F18B8E-F82B-4641-8E03-2514981C1209}">
+    <text>Fawad Ali</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64AD9EBE-916B-44FF-B78D-30B63C4E6469}">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FFB128-7185-45DB-9774-8BE493C2C42E}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -532,7 +789,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -540,7 +797,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -548,7 +805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -556,7 +813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -564,7 +821,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -572,7 +829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -580,15 +837,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -596,12 +853,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -612,7 +869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DB2185-0E3C-4BE5-BD3F-1BFF659687AF}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -620,13 +877,13 @@
       <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -634,7 +891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -642,31 +899,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -674,7 +931,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -682,23 +939,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -706,7 +963,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -714,7 +971,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -722,7 +979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -730,15 +987,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -755,15 +1012,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255">
@@ -822,9 +1070,9 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010042F0EEFC51374E449569A1D7EE9E03E1" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f6fe47d03a198c1fbfb51d8f6832cd45">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b6e6b88c-8d12-40de-97ca-53d6a0947b55" xmlns:ns3="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3205387083a8711250c9ab547032f400" ns2:_="" ns3:_="">
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010042F0EEFC51374E449569A1D7EE9E03E1" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="70735799dd56c1ee8da7f68f05dd2622">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b6e6b88c-8d12-40de-97ca-53d6a0947b55" xmlns:ns3="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="841785fd5fa88f47945d964072be431f" ns2:_="" ns3:_="">
     <xsd:import namespace="b6e6b88c-8d12-40de-97ca-53d6a0947b55"/>
     <xsd:import namespace="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255"/>
     <xsd:element name="properties">
@@ -843,6 +1091,9 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -893,6 +1144,23 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="18" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="19" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1025,39 +1293,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC31AB97-46D5-4FEB-9391-03C657BC4DCE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27287F92-5990-45D2-9430-8EC47D151C4F}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27287F92-5990-45D2-9430-8EC47D151C4F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6D94E75B-3A03-44A2-92F1-B08D451558FB}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60A4FA7D-2332-467E-A61F-E24FCB3AB047}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b6e6b88c-8d12-40de-97ca-53d6a0947b55"/>
-    <ds:schemaRef ds:uri="bacd1cd2-1dd3-4f11-98e6-3c5dee1c3255"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC31AB97-46D5-4FEB-9391-03C657BC4DCE}"/>
 </file>
</xml_diff>